<commit_message>
added calculation: covtype הרכב מינים
</commit_message>
<xml_diff>
--- a/DesheTools/configuration/fields.xlsx
+++ b/DesheTools/configuration/fields.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dedi\Desktop\עבודה\My GIS\דשא\מרץ 2024\עבודה\configuration\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dedi\Desktop\עבודה\My GIS\דשא\Github - Deshe\Deshe\DesheTools\configuration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{617B3EF0-0290-4F95-9415-4244EB06EE91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8340A3F2-FD3D-4528-9F69-DFBB5C1B8871}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" tabRatio="673" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="673" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="fields" sheetId="1" r:id="rId1"/>
@@ -27352,8 +27352,8 @@
   </sheetPr>
   <dimension ref="A1:J294"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A166" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D196" sqref="D196"/>
+    <sheetView tabSelected="1" topLeftCell="A162" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D172" sqref="D172:J178"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -33251,7 +33251,9 @@
         <f>IF(VLOOKUP($A196,fields[[code]:[length]],7,FALSE)=0, "", VLOOKUP($A196,fields[[code]:[length]],7,FALSE))</f>
         <v>50</v>
       </c>
-      <c r="J196" s="82"/>
+      <c r="J196" s="82">
+        <v>1</v>
+      </c>
     </row>
     <row r="197" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A197" s="70">
@@ -33281,7 +33283,9 @@
         <f>IF(VLOOKUP($A197,fields[[code]:[length]],7,FALSE)=0, "", VLOOKUP($A197,fields[[code]:[length]],7,FALSE))</f>
         <v>50</v>
       </c>
-      <c r="J197" s="82"/>
+      <c r="J197" s="82">
+        <v>1</v>
+      </c>
     </row>
     <row r="198" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A198" s="70">
@@ -36408,7 +36412,7 @@
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" sort="0" autoFilter="0"/>
-  <dataValidations disablePrompts="1" count="2">
+  <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H294" xr:uid="{D60CB8A1-79E7-4DD2-8B39-F4EA114A1B45}">
       <formula1>"blank,keepValues"</formula1>
     </dataValidation>

</xml_diff>

<commit_message>
fixed section "NaturalValues" (field 50075)
</commit_message>
<xml_diff>
--- a/DesheTools/configuration/fields.xlsx
+++ b/DesheTools/configuration/fields.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dedi\Desktop\עבודה\My GIS\דשא\Github - Deshe\Deshe\DesheTools\configuration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8340A3F2-FD3D-4528-9F69-DFBB5C1B8871}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63EBF9AF-A7DC-4226-92BB-9F8DF2E2388C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="673" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27352,8 +27352,8 @@
   </sheetPr>
   <dimension ref="A1:J294"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A162" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D172" sqref="D172:J178"/>
+    <sheetView tabSelected="1" topLeftCell="A236" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A246" sqref="A246"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Update script to round area values and report updated feature count
Replaced integer-based area calculation with rounding to two decimal places for improved precision (using round(..., 2)).
- Added a counter to track how many features were updated during the area calculation process
</commit_message>
<xml_diff>
--- a/DesheTools/configuration/fields.xlsx
+++ b/DesheTools/configuration/fields.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tauex-my.sharepoint.com/personal/kerenha_tauex_tau_ac_il/Documents/Documents/ArcGIS/Deshe/Deshe/DesheTools/configuration/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\galisraeli\Documents\GitHub\Deshe\DesheTools\configuration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="11" documentId="13_ncr:1_{63EBF9AF-A7DC-4226-92BB-9F8DF2E2388C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D776B01F-FA2E-46CA-87AC-A766895B2A2D}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9164DC82-2980-4F2D-899C-A4C545FDCAB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="673" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="642" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="fields" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'_fields old'!$A$1:$J$275</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">fields!$A$1:$G$294</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">fields!$A$1:$G$296</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2877" uniqueCount="492">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2947" uniqueCount="509">
   <si>
     <t>OBJECTID</t>
   </si>
@@ -1539,6 +1539,57 @@
   <si>
     <t>מקור ההצעה</t>
   </si>
+  <si>
+    <t>suggestions_after_disscusion</t>
+  </si>
+  <si>
+    <t>הערה</t>
+  </si>
+  <si>
+    <t>Stand_Number_1</t>
+  </si>
+  <si>
+    <t>Text</t>
+  </si>
+  <si>
+    <t>Stand_Number_2</t>
+  </si>
+  <si>
+    <t>Accept</t>
+  </si>
+  <si>
+    <t>For_Num</t>
+  </si>
+  <si>
+    <t>COMMENT_KKL</t>
+  </si>
+  <si>
+    <t>הערות-קק"ל</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>originStand1</t>
+  </si>
+  <si>
+    <t>עומד מקור 1</t>
+  </si>
+  <si>
+    <t>עומד מקור 2</t>
+  </si>
+  <si>
+    <t>originStand2</t>
+  </si>
+  <si>
+    <t>החלטת איחוד</t>
+  </si>
+  <si>
+    <t>CoverTypeName</t>
+  </si>
+  <si>
+    <t>COV_TYPE_CODE</t>
+  </si>
 </sst>
 </file>
 
@@ -2741,8 +2792,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E43E37A3-7B67-4000-A29A-CE671685306A}" name="fields" displayName="fields" ref="A1:G294" totalsRowShown="0" dataDxfId="63">
-  <autoFilter ref="A1:G294" xr:uid="{E43E37A3-7B67-4000-A29A-CE671685306A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E43E37A3-7B67-4000-A29A-CE671685306A}" name="fields" displayName="fields" ref="A1:G296" totalsRowShown="0" dataDxfId="63">
+  <autoFilter ref="A1:G296" xr:uid="{E43E37A3-7B67-4000-A29A-CE671685306A}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{55F41C63-F033-407F-8E01-E15B9BD574B1}" name="code" dataDxfId="62"/>
     <tableColumn id="5" xr3:uid="{1B1F22C4-6894-4A74-B995-BF7E12179554}" name="tableName(notinuse)" dataDxfId="61"/>
@@ -2757,8 +2808,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{9AC58631-8B18-47DD-880B-CB14E18DB306}" name="classification" displayName="classification" ref="A1:J294" totalsRowShown="0" headerRowDxfId="55" dataDxfId="54">
-  <autoFilter ref="A1:J294" xr:uid="{2B6FDA2F-EAB7-4D8A-BE34-7EA2F7A30E79}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{9AC58631-8B18-47DD-880B-CB14E18DB306}" name="classification" displayName="classification" ref="A1:J296" totalsRowShown="0" headerRowDxfId="55" dataDxfId="54">
+  <autoFilter ref="A1:J296" xr:uid="{2B6FDA2F-EAB7-4D8A-BE34-7EA2F7A30E79}"/>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{BE458E66-ADDE-4F2F-A00C-3B8D36E6DA4C}" name="code" dataDxfId="53"/>
     <tableColumn id="2" xr3:uid="{2F52A7D4-F3EF-4C11-8E0E-3586433181E0}" name="tableName(notinuse)" dataDxfId="52">
@@ -2788,8 +2839,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2B6FDA2F-EAB7-4D8A-BE34-7EA2F7A30E79}" name="unitePoints" displayName="unitePoints" ref="A1:J294" totalsRowShown="0" headerRowDxfId="43" dataDxfId="42">
-  <autoFilter ref="A1:J294" xr:uid="{2B6FDA2F-EAB7-4D8A-BE34-7EA2F7A30E79}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2B6FDA2F-EAB7-4D8A-BE34-7EA2F7A30E79}" name="unitePoints" displayName="unitePoints" ref="A1:J296" totalsRowShown="0" headerRowDxfId="43" dataDxfId="42">
+  <autoFilter ref="A1:J296" xr:uid="{2B6FDA2F-EAB7-4D8A-BE34-7EA2F7A30E79}"/>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{2C64E246-222E-4FD9-92A3-FEFF1E29FA2B}" name="code" dataDxfId="41"/>
     <tableColumn id="2" xr3:uid="{72F4D841-AAAC-4E6A-902A-8537D0B6E805}" name="tableName(notinuse)" dataDxfId="40">
@@ -2819,8 +2870,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{1661F715-A211-4C96-A960-ADBFF8EA9DD9}" name="unitePoints7" displayName="unitePoints7" ref="A1:J294" totalsRowShown="0" headerRowDxfId="31" dataDxfId="30">
-  <autoFilter ref="A1:J294" xr:uid="{2B6FDA2F-EAB7-4D8A-BE34-7EA2F7A30E79}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{1661F715-A211-4C96-A960-ADBFF8EA9DD9}" name="unitePoints7" displayName="unitePoints7" ref="A1:J296" totalsRowShown="0" headerRowDxfId="31" dataDxfId="30">
+  <autoFilter ref="A1:J296" xr:uid="{2B6FDA2F-EAB7-4D8A-BE34-7EA2F7A30E79}"/>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{55926AB5-993E-4EBA-B5DA-EB98B8D6A123}" name="code" dataDxfId="29"/>
     <tableColumn id="2" xr3:uid="{8E565567-253B-49B1-8313-CBA7C85855CC}" name="tableName(notinuse)" dataDxfId="28">
@@ -2850,8 +2901,8 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{301D9E6D-1BC7-4DED-BA24-E60C04C2B7D5}" name="totalCover" displayName="totalCover" ref="A1:J294" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
-  <autoFilter ref="A1:J294" xr:uid="{2B6FDA2F-EAB7-4D8A-BE34-7EA2F7A30E79}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{301D9E6D-1BC7-4DED-BA24-E60C04C2B7D5}" name="totalCover" displayName="totalCover" ref="A1:J296" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
+  <autoFilter ref="A1:J296" xr:uid="{2B6FDA2F-EAB7-4D8A-BE34-7EA2F7A30E79}"/>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{FE8A790A-3FC4-460D-A254-7F0D5B774BA6}" name="code" dataDxfId="17"/>
     <tableColumn id="2" xr3:uid="{9F0EE6CE-8ABA-45A9-8FFE-24DA4FB02269}" name="tableName(notinuse)" dataDxfId="16">
@@ -3214,19 +3265,19 @@
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A254" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F294" sqref="F294"/>
+      <selection pane="bottomLeft" activeCell="D294" sqref="D294"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.7265625" style="16"/>
-    <col min="2" max="2" width="27.81640625" style="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.453125" style="44" customWidth="1"/>
-    <col min="4" max="4" width="31.1796875" style="16" customWidth="1"/>
-    <col min="5" max="5" width="19.1796875" style="16" customWidth="1"/>
-    <col min="6" max="6" width="25.7265625" style="16" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.7265625" style="46" customWidth="1"/>
-    <col min="8" max="16384" width="8.7265625" style="16"/>
+    <col min="1" max="1" width="8.6640625" style="16"/>
+    <col min="2" max="2" width="27.88671875" style="16" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.44140625" style="44" customWidth="1"/>
+    <col min="4" max="4" width="31.109375" style="16" customWidth="1"/>
+    <col min="5" max="5" width="19.109375" style="16" customWidth="1"/>
+    <col min="6" max="6" width="25.6640625" style="16" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.6640625" style="46" customWidth="1"/>
+    <col min="8" max="16384" width="8.6640625" style="16"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
@@ -5203,7 +5254,7 @@
       <c r="F102" s="19"/>
       <c r="G102" s="19"/>
     </row>
-    <row r="103" spans="1:7" s="20" customFormat="1" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:7" s="20" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A103" s="17">
         <v>40101</v>
       </c>
@@ -5279,7 +5330,7 @@
       <c r="F106" s="19"/>
       <c r="G106" s="19"/>
     </row>
-    <row r="107" spans="1:7" s="20" customFormat="1" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:7" s="20" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A107" s="33">
         <v>40105</v>
       </c>
@@ -5355,7 +5406,7 @@
       <c r="F110" s="19"/>
       <c r="G110" s="19"/>
     </row>
-    <row r="111" spans="1:7" s="20" customFormat="1" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:7" s="20" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A111" s="33">
         <v>40109</v>
       </c>
@@ -6491,7 +6542,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="169" spans="1:7" ht="14.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:7" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A169" s="43">
         <v>50001</v>
       </c>
@@ -6508,7 +6559,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="170" spans="1:7" ht="14.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:7" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A170" s="43">
         <v>50024</v>
       </c>
@@ -6525,7 +6576,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="171" spans="1:7" ht="14.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:7" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A171" s="43">
         <v>50092</v>
       </c>
@@ -6542,7 +6593,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="172" spans="1:7" ht="12.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:7" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A172" s="43">
         <v>50093</v>
       </c>
@@ -6562,7 +6613,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="173" spans="1:7" ht="12.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:7" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A173" s="43">
         <v>50107</v>
       </c>
@@ -6580,7 +6631,7 @@
       </c>
       <c r="G173" s="51"/>
     </row>
-    <row r="174" spans="1:7" ht="12.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:7" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A174" s="43">
         <v>50094</v>
       </c>
@@ -6600,7 +6651,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="175" spans="1:7" ht="12.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:7" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A175" s="43">
         <v>50095</v>
       </c>
@@ -6620,7 +6671,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="176" spans="1:7" ht="14.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:7" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A176" s="43">
         <v>50096</v>
       </c>
@@ -6640,7 +6691,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="177" spans="1:7" ht="14.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:7" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A177" s="43">
         <v>50097</v>
       </c>
@@ -6660,7 +6711,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="178" spans="1:7" ht="14.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:7" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A178" s="43">
         <v>50080</v>
       </c>
@@ -6680,7 +6731,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="179" spans="1:7" ht="14.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:7" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A179" s="43">
         <v>50002</v>
       </c>
@@ -6714,7 +6765,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="181" spans="1:7" ht="14.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:7" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A181" s="43">
         <v>50004</v>
       </c>
@@ -6752,7 +6803,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="183" spans="1:7" ht="12.65" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:7" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A183" s="43">
         <v>50027</v>
       </c>
@@ -6769,7 +6820,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="184" spans="1:7" ht="12.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:7" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A184" s="43">
         <v>50081</v>
       </c>
@@ -6786,7 +6837,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="185" spans="1:7" ht="12.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:7" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A185" s="43">
         <v>50098</v>
       </c>
@@ -6806,7 +6857,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="186" spans="1:7" ht="12.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:7" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A186" s="43">
         <v>50099</v>
       </c>
@@ -6827,7 +6878,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="187" spans="1:7" ht="12.65" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:7" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A187" s="43">
         <v>50028</v>
       </c>
@@ -6850,7 +6901,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="188" spans="1:7" ht="12.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:7" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A188" s="43">
         <v>50082</v>
       </c>
@@ -6870,7 +6921,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="189" spans="1:7" ht="12.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:7" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A189" s="43">
         <v>50083</v>
       </c>
@@ -6890,7 +6941,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="190" spans="1:7" s="59" customFormat="1" ht="12.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:7" s="59" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A190" s="43">
         <v>50084</v>
       </c>
@@ -6911,7 +6962,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="191" spans="1:7" ht="12.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:7" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A191" s="43">
         <v>50086</v>
       </c>
@@ -6928,7 +6979,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="192" spans="1:7" ht="12.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:7" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A192" s="43">
         <v>50085</v>
       </c>
@@ -6945,7 +6996,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="193" spans="1:7" ht="12.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:7" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A193" s="43">
         <v>50100</v>
       </c>
@@ -6965,7 +7016,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="194" spans="1:7" ht="12.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:7" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A194" s="43">
         <v>50015</v>
       </c>
@@ -6985,7 +7036,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="195" spans="1:7" ht="12.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:7" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A195" s="43">
         <v>50087</v>
       </c>
@@ -7002,7 +7053,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="196" spans="1:7" ht="12.65" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:7" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A196" s="43">
         <v>50039</v>
       </c>
@@ -7025,7 +7076,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="197" spans="1:7" ht="12.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:7" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A197" s="43">
         <v>50038</v>
       </c>
@@ -7048,7 +7099,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="198" spans="1:7" ht="12.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:7" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A198" s="43">
         <v>50040</v>
       </c>
@@ -7068,7 +7119,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="199" spans="1:7" ht="12.65" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:7" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A199" s="43">
         <v>50037</v>
       </c>
@@ -7091,7 +7142,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="200" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:7" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A200" s="43">
         <v>50041</v>
       </c>
@@ -7114,7 +7165,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="201" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:7" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A201" s="43">
         <v>50045</v>
       </c>
@@ -7137,7 +7188,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="202" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:7" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A202" s="43">
         <v>50042</v>
       </c>
@@ -7160,7 +7211,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="203" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:7" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A203" s="43">
         <v>50044</v>
       </c>
@@ -7183,7 +7234,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="204" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:7" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A204" s="43">
         <v>50088</v>
       </c>
@@ -7206,7 +7257,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="205" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:7" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A205" s="43">
         <v>50043</v>
       </c>
@@ -7229,7 +7280,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="206" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:7" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A206" s="43">
         <v>50032</v>
       </c>
@@ -7249,7 +7300,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="207" spans="1:7" ht="13" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A207" s="43">
         <v>50030</v>
       </c>
@@ -7272,7 +7323,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="208" spans="1:7" ht="13" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A208" s="43">
         <v>50029</v>
       </c>
@@ -7295,7 +7346,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="209" spans="1:7" ht="13" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A209" s="43">
         <v>50031</v>
       </c>
@@ -7318,7 +7369,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="210" spans="1:7" ht="13" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A210" s="43">
         <v>50036</v>
       </c>
@@ -7338,7 +7389,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="211" spans="1:7" ht="13" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A211" s="43">
         <v>50034</v>
       </c>
@@ -7361,7 +7412,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="212" spans="1:7" ht="13" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A212" s="43">
         <v>50033</v>
       </c>
@@ -7384,7 +7435,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="213" spans="1:7" ht="13" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A213" s="43">
         <v>50035</v>
       </c>
@@ -7407,7 +7458,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="214" spans="1:7" ht="13" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A214" s="43">
         <v>50046</v>
       </c>
@@ -7427,7 +7478,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="215" spans="1:7" ht="13" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A215" s="43">
         <v>50047</v>
       </c>
@@ -7450,7 +7501,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="216" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A216" s="43">
         <v>50049</v>
       </c>
@@ -7470,7 +7521,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="217" spans="1:7" ht="13" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A217" s="43">
         <v>50048</v>
       </c>
@@ -7490,7 +7541,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="218" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:7" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A218" s="43">
         <v>50050</v>
       </c>
@@ -7510,7 +7561,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="219" spans="1:7" ht="13" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A219" s="43">
         <v>50051</v>
       </c>
@@ -7533,7 +7584,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="220" spans="1:7" ht="13" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A220" s="43">
         <v>50053</v>
       </c>
@@ -7553,7 +7604,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="221" spans="1:7" ht="13" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A221" s="43">
         <v>50052</v>
       </c>
@@ -7573,7 +7624,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="222" spans="1:7" ht="13" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A222" s="43">
         <v>50054</v>
       </c>
@@ -7593,7 +7644,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="223" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:7" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A223" s="43">
         <v>50055</v>
       </c>
@@ -7616,7 +7667,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="224" spans="1:7" ht="13" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A224" s="43">
         <v>50057</v>
       </c>
@@ -7636,7 +7687,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="225" spans="1:7" ht="13" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A225" s="43">
         <v>50056</v>
       </c>
@@ -7656,7 +7707,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="226" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:7" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A226" s="43">
         <v>50058</v>
       </c>
@@ -7676,7 +7727,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="227" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:7" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A227" s="43">
         <v>50089</v>
       </c>
@@ -7699,7 +7750,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="228" spans="1:7" ht="13" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A228" s="43">
         <v>50060</v>
       </c>
@@ -7719,7 +7770,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="229" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:7" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A229" s="43">
         <v>50059</v>
       </c>
@@ -7739,7 +7790,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="230" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:7" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A230" s="43">
         <v>50061</v>
       </c>
@@ -7759,7 +7810,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="231" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:7" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A231" s="43">
         <v>50062</v>
       </c>
@@ -7779,7 +7830,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="232" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:7" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A232" s="43">
         <v>50063</v>
       </c>
@@ -7802,7 +7853,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="233" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:7" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A233" s="43">
         <v>50064</v>
       </c>
@@ -7825,7 +7876,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="234" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:7" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A234" s="43">
         <v>50065</v>
       </c>
@@ -7848,7 +7899,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="235" spans="1:7" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:7" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A235" s="43">
         <v>50066</v>
       </c>
@@ -7871,7 +7922,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="236" spans="1:7" ht="13" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A236" s="43">
         <v>50102</v>
       </c>
@@ -7891,7 +7942,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="237" spans="1:7" ht="13" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A237" s="43">
         <v>50068</v>
       </c>
@@ -7914,7 +7965,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="238" spans="1:7" ht="13" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A238" s="43">
         <v>50069</v>
       </c>
@@ -7937,7 +7988,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="239" spans="1:7" ht="13" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A239" s="43">
         <v>50070</v>
       </c>
@@ -7960,7 +8011,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="240" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:7" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A240" s="43">
         <v>50071</v>
       </c>
@@ -7983,7 +8034,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="241" spans="1:7" ht="13" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A241" s="43">
         <v>50067</v>
       </c>
@@ -8006,7 +8057,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="242" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:7" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A242" s="43">
         <v>50072</v>
       </c>
@@ -8029,7 +8080,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="243" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:7" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A243" s="43">
         <v>50073</v>
       </c>
@@ -8049,7 +8100,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="244" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:7" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A244" s="43">
         <v>50074</v>
       </c>
@@ -8069,7 +8120,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="245" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:7" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A245" s="43">
         <v>50075</v>
       </c>
@@ -8090,7 +8141,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="246" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:7" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A246" s="43">
         <v>50103</v>
       </c>
@@ -8111,7 +8162,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="247" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:7" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A247" s="43">
         <v>50076</v>
       </c>
@@ -8131,7 +8182,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="248" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:7" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A248" s="43">
         <v>50104</v>
       </c>
@@ -8151,7 +8202,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="249" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:7" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A249" s="43">
         <v>50077</v>
       </c>
@@ -8171,7 +8222,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="250" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:7" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A250" s="43">
         <v>50105</v>
       </c>
@@ -8191,7 +8242,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="251" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:7" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A251" s="43">
         <v>50078</v>
       </c>
@@ -8211,7 +8262,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="252" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:7" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A252" s="43">
         <v>50106</v>
       </c>
@@ -8231,7 +8282,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="253" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:7" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A253" s="43">
         <v>50091</v>
       </c>
@@ -8251,7 +8302,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="254" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:7" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A254" s="43">
         <v>50079</v>
       </c>
@@ -8271,7 +8322,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="255" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:7" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A255" s="43">
         <v>50101</v>
       </c>
@@ -8292,7 +8343,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="256" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:7" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A256" s="43">
         <v>50000</v>
       </c>
@@ -8610,7 +8661,7 @@
       <c r="F273" s="16"/>
       <c r="G273" s="46"/>
     </row>
-    <row r="274" spans="1:7" s="20" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:7" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A274" s="65">
         <v>59000</v>
       </c>
@@ -8627,7 +8678,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="275" spans="1:7" s="20" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:7" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A275" s="65">
         <f>A274+1</f>
         <v>59001</v>
@@ -8645,7 +8696,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="276" spans="1:7" s="20" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:7" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A276" s="65">
         <f>A275+1</f>
         <v>59002</v>
@@ -8663,7 +8714,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="277" spans="1:7" s="20" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:7" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A277" s="65">
         <f>A276+1</f>
         <v>59003</v>
@@ -8681,7 +8732,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="278" spans="1:7" s="20" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:7" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A278" s="65">
         <f>A277+1</f>
         <v>59004</v>
@@ -8699,7 +8750,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="279" spans="1:7" s="20" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:7" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A279" s="65">
         <f>A278+1</f>
         <v>59005</v>
@@ -8779,7 +8830,7 @@
       </c>
       <c r="G282" s="20"/>
     </row>
-    <row r="283" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:7" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A283" s="39">
         <f>A282+1</f>
         <v>52002</v>
@@ -8822,7 +8873,7 @@
       </c>
       <c r="G284" s="20"/>
     </row>
-    <row r="285" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:7" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A285" s="40">
         <f>A284+1</f>
         <v>53002</v>
@@ -8844,7 +8895,7 @@
       </c>
       <c r="G285" s="20"/>
     </row>
-    <row r="286" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:7" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A286" s="41">
         <v>54001</v>
       </c>
@@ -8865,7 +8916,7 @@
       </c>
       <c r="G286" s="20"/>
     </row>
-    <row r="287" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:7" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A287" s="41">
         <f>A286+1</f>
         <v>54002</v>
@@ -9003,7 +9054,7 @@
         <v>428</v>
       </c>
       <c r="D294" s="16" t="s">
-        <v>429</v>
+        <v>506</v>
       </c>
       <c r="E294" s="16" t="s">
         <v>14</v>
@@ -9013,19 +9064,42 @@
       </c>
     </row>
     <row r="295" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A295"/>
-      <c r="B295"/>
-      <c r="C295"/>
+      <c r="A295" s="43">
+        <v>60007</v>
+      </c>
+      <c r="B295" s="36" t="s">
+        <v>426</v>
+      </c>
+      <c r="C295" s="44" t="s">
+        <v>502</v>
+      </c>
+      <c r="D295" s="16" t="s">
+        <v>503</v>
+      </c>
+      <c r="E295" s="20" t="s">
+        <v>212</v>
+      </c>
     </row>
     <row r="296" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A296"/>
-      <c r="B296"/>
-      <c r="C296"/>
+      <c r="A296" s="70">
+        <v>60008</v>
+      </c>
+      <c r="B296" s="36" t="s">
+        <v>426</v>
+      </c>
+      <c r="C296" s="44" t="s">
+        <v>505</v>
+      </c>
+      <c r="D296" s="16" t="s">
+        <v>504</v>
+      </c>
+      <c r="E296" s="20" t="s">
+        <v>212</v>
+      </c>
     </row>
     <row r="297" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A297"/>
-      <c r="B297"/>
-      <c r="C297"/>
+      <c r="B297" s="36"/>
     </row>
     <row r="298" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A298"/>
@@ -9081,28 +9155,28 @@
   <sheetPr codeName="Sheet3">
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
-  <dimension ref="A1:J294"/>
+  <dimension ref="A1:J296"/>
   <sheetViews>
-    <sheetView topLeftCell="A100" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A117" sqref="A117"/>
+    <sheetView topLeftCell="A271" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A298" sqref="A298"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.1796875" style="71"/>
-    <col min="2" max="2" width="30.26953125" style="69" customWidth="1"/>
-    <col min="3" max="3" width="26.7265625" style="69" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="41.453125" style="69" customWidth="1"/>
-    <col min="5" max="5" width="9.1796875" style="69"/>
-    <col min="6" max="6" width="25.26953125" style="69" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.1796875" style="69"/>
-    <col min="8" max="8" width="13.26953125" style="20" customWidth="1"/>
-    <col min="9" max="9" width="14.1796875" style="20" customWidth="1"/>
-    <col min="10" max="10" width="17.54296875" style="20" customWidth="1"/>
-    <col min="11" max="16384" width="9.1796875" style="20"/>
+    <col min="1" max="1" width="9.109375" style="71"/>
+    <col min="2" max="2" width="30.33203125" style="69" customWidth="1"/>
+    <col min="3" max="3" width="26.6640625" style="69" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="41.44140625" style="69" customWidth="1"/>
+    <col min="5" max="5" width="9.109375" style="69"/>
+    <col min="6" max="6" width="25.33203125" style="69" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.109375" style="69"/>
+    <col min="8" max="8" width="13.33203125" style="20" customWidth="1"/>
+    <col min="9" max="9" width="14.109375" style="20" customWidth="1"/>
+    <col min="10" max="10" width="17.5546875" style="20" customWidth="1"/>
+    <col min="11" max="16384" width="9.109375" style="20"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -12249,7 +12323,7 @@
       </c>
       <c r="J102" s="82"/>
     </row>
-    <row r="103" spans="1:10" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:10" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A103" s="2">
         <v>40101</v>
       </c>
@@ -12375,7 +12449,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="107" spans="1:10" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:10" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A107" s="9">
         <v>40105</v>
       </c>
@@ -12503,7 +12577,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="111" spans="1:10" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:10" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A111" s="9">
         <v>40109</v>
       </c>
@@ -14045,7 +14119,7 @@
       </c>
       <c r="J160" s="82"/>
     </row>
-    <row r="161" spans="1:10" ht="13" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A161" s="4">
         <v>44002</v>
       </c>
@@ -14074,7 +14148,7 @@
         <v/>
       </c>
     </row>
-    <row r="162" spans="1:10" ht="13" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A162" s="4">
         <v>44003</v>
       </c>
@@ -17433,7 +17507,7 @@
       </c>
       <c r="J273" s="82"/>
     </row>
-    <row r="274" spans="1:10" ht="13" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A274" s="11">
         <v>59000</v>
       </c>
@@ -17463,7 +17537,7 @@
       </c>
       <c r="J274" s="82"/>
     </row>
-    <row r="275" spans="1:10" ht="13" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A275" s="11">
         <f>A274+1</f>
         <v>59001</v>
@@ -17494,7 +17568,7 @@
       </c>
       <c r="J275" s="82"/>
     </row>
-    <row r="276" spans="1:10" ht="13" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A276" s="11">
         <f>A275+1</f>
         <v>59002</v>
@@ -17525,7 +17599,7 @@
       </c>
       <c r="J276" s="82"/>
     </row>
-    <row r="277" spans="1:10" ht="13" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A277" s="11">
         <f>A276+1</f>
         <v>59003</v>
@@ -17556,7 +17630,7 @@
       </c>
       <c r="J277" s="82"/>
     </row>
-    <row r="278" spans="1:10" ht="13" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A278" s="11">
         <f>A277+1</f>
         <v>59004</v>
@@ -17587,7 +17661,7 @@
       </c>
       <c r="J278" s="82"/>
     </row>
-    <row r="279" spans="1:10" ht="13" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A279" s="11">
         <f>A278+1</f>
         <v>59005</v>
@@ -18050,7 +18124,7 @@
       </c>
       <c r="D294" s="92" t="str">
         <f>IF(VLOOKUP($A294,fields[[code]:[length]],4,FALSE)=0, "", VLOOKUP($A294,fields[[code]:[length]],4,FALSE))</f>
-        <v>החלטה</v>
+        <v>החלטת איחוד</v>
       </c>
       <c r="E294" s="92" t="str">
         <f>IF(VLOOKUP($A294,fields[[code]:[length]],5,FALSE)=0, "", VLOOKUP($A294,fields[[code]:[length]],5,FALSE))</f>
@@ -18067,6 +18141,64 @@
       <c r="H294" s="20"/>
       <c r="I294" s="20"/>
       <c r="J294" s="20"/>
+    </row>
+    <row r="295" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A295" s="43">
+        <v>60007</v>
+      </c>
+      <c r="B295" s="92" t="str">
+        <f>IF(VLOOKUP($A295,fields[[code]:[length]],2,FALSE)=0, "", VLOOKUP($A295,fields[[code]:[length]],2,FALSE))</f>
+        <v>unite lines</v>
+      </c>
+      <c r="C295" s="92" t="str">
+        <f>IF(VLOOKUP($A295,fields[[code]:[length]],3,FALSE)=0, "", VLOOKUP($A295,fields[[code]:[length]],3,FALSE))</f>
+        <v>originStand1</v>
+      </c>
+      <c r="D295" s="92" t="str">
+        <f>IF(VLOOKUP($A295,fields[[code]:[length]],4,FALSE)=0, "", VLOOKUP($A295,fields[[code]:[length]],4,FALSE))</f>
+        <v>עומד מקור 1</v>
+      </c>
+      <c r="E295" s="92" t="str">
+        <f>IF(VLOOKUP($A295,fields[[code]:[length]],5,FALSE)=0, "", VLOOKUP($A295,fields[[code]:[length]],5,FALSE))</f>
+        <v>Guid</v>
+      </c>
+      <c r="F295" s="92" t="str">
+        <f>IF(VLOOKUP($A295,fields[[code]:[length]],6,FALSE)=0, "", VLOOKUP($A295,fields[[code]:[length]],6,FALSE))</f>
+        <v/>
+      </c>
+      <c r="G295" s="92" t="str">
+        <f>IF(VLOOKUP($A295,fields[[code]:[length]],7,FALSE)=0, "", VLOOKUP($A295,fields[[code]:[length]],7,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="296" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A296" s="70">
+        <v>60008</v>
+      </c>
+      <c r="B296" s="92" t="str">
+        <f>IF(VLOOKUP($A296,fields[[code]:[length]],2,FALSE)=0, "", VLOOKUP($A296,fields[[code]:[length]],2,FALSE))</f>
+        <v>unite lines</v>
+      </c>
+      <c r="C296" s="92" t="str">
+        <f>IF(VLOOKUP($A296,fields[[code]:[length]],3,FALSE)=0, "", VLOOKUP($A296,fields[[code]:[length]],3,FALSE))</f>
+        <v>originStand2</v>
+      </c>
+      <c r="D296" s="92" t="str">
+        <f>IF(VLOOKUP($A296,fields[[code]:[length]],4,FALSE)=0, "", VLOOKUP($A296,fields[[code]:[length]],4,FALSE))</f>
+        <v>עומד מקור 2</v>
+      </c>
+      <c r="E296" s="92" t="str">
+        <f>IF(VLOOKUP($A296,fields[[code]:[length]],5,FALSE)=0, "", VLOOKUP($A296,fields[[code]:[length]],5,FALSE))</f>
+        <v>Guid</v>
+      </c>
+      <c r="F296" s="92" t="str">
+        <f>IF(VLOOKUP($A296,fields[[code]:[length]],6,FALSE)=0, "", VLOOKUP($A296,fields[[code]:[length]],6,FALSE))</f>
+        <v/>
+      </c>
+      <c r="G296" s="92" t="str">
+        <f>IF(VLOOKUP($A296,fields[[code]:[length]],7,FALSE)=0, "", VLOOKUP($A296,fields[[code]:[length]],7,FALSE))</f>
+        <v/>
+      </c>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" sort="0" autoFilter="0"/>
@@ -18076,10 +18208,10 @@
       <formula1>0</formula1>
       <formula2>9999999999</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J294" xr:uid="{161D6BE2-4DE6-4553-9FC5-78D751EC8A60}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J296" xr:uid="{161D6BE2-4DE6-4553-9FC5-78D751EC8A60}">
       <formula1>"1"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H294" xr:uid="{AE126A03-27E1-47EF-9753-850F0D3FBDA1}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H296" xr:uid="{AE126A03-27E1-47EF-9753-850F0D3FBDA1}">
       <formula1>"blank,keepValues"</formula1>
     </dataValidation>
   </dataValidations>
@@ -18096,28 +18228,28 @@
   <sheetPr codeName="Sheet2">
     <tabColor rgb="FF00B050"/>
   </sheetPr>
-  <dimension ref="A1:J294"/>
+  <dimension ref="A1:J296"/>
   <sheetViews>
-    <sheetView topLeftCell="A92" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A117" sqref="A117"/>
+    <sheetView topLeftCell="A264" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A295" sqref="A295:A296"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.7265625" style="71" customWidth="1"/>
-    <col min="2" max="2" width="27.81640625" style="69" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.7265625" style="69" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="41.453125" style="69" customWidth="1"/>
-    <col min="5" max="5" width="9.1796875" style="69"/>
-    <col min="6" max="6" width="25.26953125" style="69" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.1796875" style="69"/>
-    <col min="8" max="8" width="10.54296875" style="20" customWidth="1"/>
-    <col min="9" max="9" width="14.1796875" style="20" customWidth="1"/>
-    <col min="10" max="10" width="17.54296875" style="20" customWidth="1"/>
-    <col min="11" max="16384" width="9.1796875" style="20"/>
+    <col min="1" max="1" width="8.6640625" style="71" customWidth="1"/>
+    <col min="2" max="2" width="27.88671875" style="69" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.6640625" style="69" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="41.44140625" style="69" customWidth="1"/>
+    <col min="5" max="5" width="9.109375" style="69"/>
+    <col min="6" max="6" width="25.33203125" style="69" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.109375" style="69"/>
+    <col min="8" max="8" width="10.5546875" style="20" customWidth="1"/>
+    <col min="9" max="9" width="14.109375" style="20" customWidth="1"/>
+    <col min="10" max="10" width="17.5546875" style="20" customWidth="1"/>
+    <col min="11" max="16384" width="9.109375" style="20"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -21246,7 +21378,7 @@
       </c>
       <c r="J102" s="82"/>
     </row>
-    <row r="103" spans="1:10" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:10" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A103" s="2">
         <v>40101</v>
       </c>
@@ -21372,7 +21504,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:10" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:10" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A107" s="9">
         <v>40105</v>
       </c>
@@ -21500,7 +21632,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:10" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:10" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A111" s="9">
         <v>40109</v>
       </c>
@@ -26912,7 +27044,7 @@
       </c>
       <c r="J273" s="82"/>
     </row>
-    <row r="274" spans="1:10" ht="13" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A274" s="11">
         <v>59000</v>
       </c>
@@ -26945,7 +27077,7 @@
       </c>
       <c r="J274" s="82"/>
     </row>
-    <row r="275" spans="1:10" ht="13" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A275" s="11">
         <f>A274+1</f>
         <v>59001</v>
@@ -26979,7 +27111,7 @@
       </c>
       <c r="J275" s="82"/>
     </row>
-    <row r="276" spans="1:10" ht="13" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A276" s="11">
         <f>A275+1</f>
         <v>59002</v>
@@ -27013,7 +27145,7 @@
       </c>
       <c r="J276" s="82"/>
     </row>
-    <row r="277" spans="1:10" ht="13" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A277" s="11">
         <f>A276+1</f>
         <v>59003</v>
@@ -27047,7 +27179,7 @@
       </c>
       <c r="J277" s="82"/>
     </row>
-    <row r="278" spans="1:10" ht="13" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A278" s="11">
         <f>A277+1</f>
         <v>59004</v>
@@ -27081,7 +27213,7 @@
       </c>
       <c r="J278" s="82"/>
     </row>
-    <row r="279" spans="1:10" ht="13" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A279" s="11">
         <f>A278+1</f>
         <v>59005</v>
@@ -27571,7 +27703,7 @@
       </c>
       <c r="D294" s="92" t="str">
         <f>IF(VLOOKUP($A294,fields[[code]:[length]],4,FALSE)=0, "", VLOOKUP($A294,fields[[code]:[length]],4,FALSE))</f>
-        <v>החלטה</v>
+        <v>החלטת איחוד</v>
       </c>
       <c r="E294" s="92" t="str">
         <f>IF(VLOOKUP($A294,fields[[code]:[length]],5,FALSE)=0, "", VLOOKUP($A294,fields[[code]:[length]],5,FALSE))</f>
@@ -27586,13 +27718,71 @@
         <v/>
       </c>
     </row>
+    <row r="295" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A295" s="43">
+        <v>60007</v>
+      </c>
+      <c r="B295" s="92" t="str">
+        <f>IF(VLOOKUP($A295,fields[[code]:[length]],2,FALSE)=0, "", VLOOKUP($A295,fields[[code]:[length]],2,FALSE))</f>
+        <v>unite lines</v>
+      </c>
+      <c r="C295" s="92" t="str">
+        <f>IF(VLOOKUP($A295,fields[[code]:[length]],3,FALSE)=0, "", VLOOKUP($A295,fields[[code]:[length]],3,FALSE))</f>
+        <v>originStand1</v>
+      </c>
+      <c r="D295" s="92" t="str">
+        <f>IF(VLOOKUP($A295,fields[[code]:[length]],4,FALSE)=0, "", VLOOKUP($A295,fields[[code]:[length]],4,FALSE))</f>
+        <v>עומד מקור 1</v>
+      </c>
+      <c r="E295" s="92" t="str">
+        <f>IF(VLOOKUP($A295,fields[[code]:[length]],5,FALSE)=0, "", VLOOKUP($A295,fields[[code]:[length]],5,FALSE))</f>
+        <v>Guid</v>
+      </c>
+      <c r="F295" s="92" t="str">
+        <f>IF(VLOOKUP($A295,fields[[code]:[length]],6,FALSE)=0, "", VLOOKUP($A295,fields[[code]:[length]],6,FALSE))</f>
+        <v/>
+      </c>
+      <c r="G295" s="92" t="str">
+        <f>IF(VLOOKUP($A295,fields[[code]:[length]],7,FALSE)=0, "", VLOOKUP($A295,fields[[code]:[length]],7,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="296" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A296" s="70">
+        <v>60008</v>
+      </c>
+      <c r="B296" s="92" t="str">
+        <f>IF(VLOOKUP($A296,fields[[code]:[length]],2,FALSE)=0, "", VLOOKUP($A296,fields[[code]:[length]],2,FALSE))</f>
+        <v>unite lines</v>
+      </c>
+      <c r="C296" s="92" t="str">
+        <f>IF(VLOOKUP($A296,fields[[code]:[length]],3,FALSE)=0, "", VLOOKUP($A296,fields[[code]:[length]],3,FALSE))</f>
+        <v>originStand2</v>
+      </c>
+      <c r="D296" s="92" t="str">
+        <f>IF(VLOOKUP($A296,fields[[code]:[length]],4,FALSE)=0, "", VLOOKUP($A296,fields[[code]:[length]],4,FALSE))</f>
+        <v>עומד מקור 2</v>
+      </c>
+      <c r="E296" s="92" t="str">
+        <f>IF(VLOOKUP($A296,fields[[code]:[length]],5,FALSE)=0, "", VLOOKUP($A296,fields[[code]:[length]],5,FALSE))</f>
+        <v>Guid</v>
+      </c>
+      <c r="F296" s="92" t="str">
+        <f>IF(VLOOKUP($A296,fields[[code]:[length]],6,FALSE)=0, "", VLOOKUP($A296,fields[[code]:[length]],6,FALSE))</f>
+        <v/>
+      </c>
+      <c r="G296" s="92" t="str">
+        <f>IF(VLOOKUP($A296,fields[[code]:[length]],7,FALSE)=0, "", VLOOKUP($A296,fields[[code]:[length]],7,FALSE))</f>
+        <v/>
+      </c>
+    </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" sort="0" autoFilter="0"/>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J294" xr:uid="{EB947E22-4305-442D-BBE3-E8B970A9AD1D}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J296" xr:uid="{EB947E22-4305-442D-BBE3-E8B970A9AD1D}">
       <formula1>"1"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H294" xr:uid="{0FF0978D-1F41-4343-9AC2-B21428233DF6}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H296" xr:uid="{0FF0978D-1F41-4343-9AC2-B21428233DF6}">
       <formula1>"blank,keepValues"</formula1>
     </dataValidation>
   </dataValidations>
@@ -27609,28 +27799,28 @@
   <sheetPr>
     <tabColor theme="5"/>
   </sheetPr>
-  <dimension ref="A1:J294"/>
+  <dimension ref="A1:J296"/>
   <sheetViews>
-    <sheetView topLeftCell="A236" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A246" sqref="A246"/>
+    <sheetView topLeftCell="A258" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F288" sqref="F288"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.1796875" style="71"/>
-    <col min="2" max="2" width="30.54296875" style="69" customWidth="1"/>
-    <col min="3" max="3" width="26.7265625" style="69" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="41.453125" style="69" customWidth="1"/>
-    <col min="5" max="5" width="9.1796875" style="69"/>
-    <col min="6" max="6" width="25.26953125" style="69" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.1796875" style="69"/>
-    <col min="8" max="8" width="10.54296875" style="20" customWidth="1"/>
-    <col min="9" max="9" width="14.1796875" style="20" customWidth="1"/>
-    <col min="10" max="10" width="17.54296875" style="20" customWidth="1"/>
-    <col min="11" max="16384" width="9.1796875" style="20"/>
+    <col min="1" max="1" width="9.109375" style="71"/>
+    <col min="2" max="2" width="30.5546875" style="69" customWidth="1"/>
+    <col min="3" max="3" width="26.6640625" style="69" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="41.44140625" style="69" customWidth="1"/>
+    <col min="5" max="5" width="9.109375" style="69"/>
+    <col min="6" max="6" width="25.33203125" style="69" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.109375" style="69"/>
+    <col min="8" max="8" width="10.5546875" style="20" customWidth="1"/>
+    <col min="9" max="9" width="14.109375" style="20" customWidth="1"/>
+    <col min="10" max="10" width="17.5546875" style="20" customWidth="1"/>
+    <col min="11" max="16384" width="9.109375" style="20"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -30688,7 +30878,7 @@
       </c>
       <c r="J102" s="82"/>
     </row>
-    <row r="103" spans="1:10" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:10" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A103" s="2">
         <v>40101</v>
       </c>
@@ -30805,7 +30995,7 @@
         <v/>
       </c>
     </row>
-    <row r="107" spans="1:10" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:10" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A107" s="9">
         <v>40105</v>
       </c>
@@ -30921,7 +31111,7 @@
         <v/>
       </c>
     </row>
-    <row r="111" spans="1:10" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:10" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A111" s="9">
         <v>40109</v>
       </c>
@@ -36008,7 +36198,7 @@
       </c>
       <c r="J273" s="82"/>
     </row>
-    <row r="274" spans="1:10" ht="13" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A274" s="11">
         <v>59000</v>
       </c>
@@ -36038,7 +36228,7 @@
       </c>
       <c r="J274" s="82"/>
     </row>
-    <row r="275" spans="1:10" ht="13" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A275" s="11">
         <v>59001</v>
       </c>
@@ -36070,7 +36260,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="276" spans="1:10" ht="13" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A276" s="11">
         <v>59002</v>
       </c>
@@ -36102,7 +36292,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="277" spans="1:10" ht="13" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A277" s="11">
         <v>59003</v>
       </c>
@@ -36134,7 +36324,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="278" spans="1:10" ht="13" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A278" s="11">
         <v>59004</v>
       </c>
@@ -36166,7 +36356,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="279" spans="1:10" ht="13" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A279" s="11">
         <v>59005</v>
       </c>
@@ -36654,7 +36844,7 @@
       </c>
       <c r="D294" s="92" t="str">
         <f>IF(VLOOKUP($A294,fields[[code]:[length]],4,FALSE)=0, "", VLOOKUP($A294,fields[[code]:[length]],4,FALSE))</f>
-        <v>החלטה</v>
+        <v>החלטת איחוד</v>
       </c>
       <c r="E294" s="92" t="str">
         <f>IF(VLOOKUP($A294,fields[[code]:[length]],5,FALSE)=0, "", VLOOKUP($A294,fields[[code]:[length]],5,FALSE))</f>
@@ -36668,14 +36858,81 @@
         <f>IF(VLOOKUP($A294,fields[[code]:[length]],7,FALSE)=0, "", VLOOKUP($A294,fields[[code]:[length]],7,FALSE))</f>
         <v/>
       </c>
+      <c r="H294" s="20" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="295" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A295" s="43">
+        <v>60007</v>
+      </c>
+      <c r="B295" s="92" t="str">
+        <f>IF(VLOOKUP($A295,fields[[code]:[length]],2,FALSE)=0, "", VLOOKUP($A295,fields[[code]:[length]],2,FALSE))</f>
+        <v>unite lines</v>
+      </c>
+      <c r="C295" s="92" t="str">
+        <f>IF(VLOOKUP($A295,fields[[code]:[length]],3,FALSE)=0, "", VLOOKUP($A295,fields[[code]:[length]],3,FALSE))</f>
+        <v>originStand1</v>
+      </c>
+      <c r="D295" s="92" t="str">
+        <f>IF(VLOOKUP($A295,fields[[code]:[length]],4,FALSE)=0, "", VLOOKUP($A295,fields[[code]:[length]],4,FALSE))</f>
+        <v>עומד מקור 1</v>
+      </c>
+      <c r="E295" s="92" t="str">
+        <f>IF(VLOOKUP($A295,fields[[code]:[length]],5,FALSE)=0, "", VLOOKUP($A295,fields[[code]:[length]],5,FALSE))</f>
+        <v>Guid</v>
+      </c>
+      <c r="F295" s="92" t="str">
+        <f>IF(VLOOKUP($A295,fields[[code]:[length]],6,FALSE)=0, "", VLOOKUP($A295,fields[[code]:[length]],6,FALSE))</f>
+        <v/>
+      </c>
+      <c r="G295" s="92" t="str">
+        <f>IF(VLOOKUP($A295,fields[[code]:[length]],7,FALSE)=0, "", VLOOKUP($A295,fields[[code]:[length]],7,FALSE))</f>
+        <v/>
+      </c>
+      <c r="H295" s="20" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="296" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A296" s="70">
+        <v>60008</v>
+      </c>
+      <c r="B296" s="92" t="str">
+        <f>IF(VLOOKUP($A296,fields[[code]:[length]],2,FALSE)=0, "", VLOOKUP($A296,fields[[code]:[length]],2,FALSE))</f>
+        <v>unite lines</v>
+      </c>
+      <c r="C296" s="92" t="str">
+        <f>IF(VLOOKUP($A296,fields[[code]:[length]],3,FALSE)=0, "", VLOOKUP($A296,fields[[code]:[length]],3,FALSE))</f>
+        <v>originStand2</v>
+      </c>
+      <c r="D296" s="92" t="str">
+        <f>IF(VLOOKUP($A296,fields[[code]:[length]],4,FALSE)=0, "", VLOOKUP($A296,fields[[code]:[length]],4,FALSE))</f>
+        <v>עומד מקור 2</v>
+      </c>
+      <c r="E296" s="92" t="str">
+        <f>IF(VLOOKUP($A296,fields[[code]:[length]],5,FALSE)=0, "", VLOOKUP($A296,fields[[code]:[length]],5,FALSE))</f>
+        <v>Guid</v>
+      </c>
+      <c r="F296" s="92" t="str">
+        <f>IF(VLOOKUP($A296,fields[[code]:[length]],6,FALSE)=0, "", VLOOKUP($A296,fields[[code]:[length]],6,FALSE))</f>
+        <v/>
+      </c>
+      <c r="G296" s="92" t="str">
+        <f>IF(VLOOKUP($A296,fields[[code]:[length]],7,FALSE)=0, "", VLOOKUP($A296,fields[[code]:[length]],7,FALSE))</f>
+        <v/>
+      </c>
+      <c r="H296" s="20" t="s">
+        <v>399</v>
+      </c>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" sort="0" autoFilter="0"/>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H294" xr:uid="{D60CB8A1-79E7-4DD2-8B39-F4EA114A1B45}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H296" xr:uid="{D60CB8A1-79E7-4DD2-8B39-F4EA114A1B45}">
       <formula1>"blank,keepValues"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J294" xr:uid="{1DED5A06-4E76-48A1-BDAF-35C528B02E5E}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J296" xr:uid="{1DED5A06-4E76-48A1-BDAF-35C528B02E5E}">
       <formula1>"1"</formula1>
     </dataValidation>
   </dataValidations>
@@ -36689,15 +36946,22 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B206E146-10D4-4101-A6FA-71BD0AF9A72C}">
-  <dimension ref="A1:J52"/>
+  <dimension ref="A1:J65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O22" sqref="O22"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="35.33203125" customWidth="1"/>
+    <col min="2" max="2" width="33.33203125" customWidth="1"/>
+    <col min="3" max="3" width="13" customWidth="1"/>
+    <col min="5" max="5" width="14.109375" customWidth="1"/>
+    <col min="10" max="10" width="9.109375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="93" t="s">
         <v>431</v>
       </c>
@@ -36871,6 +37135,9 @@
       <c r="I9">
         <v>1</v>
       </c>
+      <c r="J9" t="s">
+        <v>471</v>
+      </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="98" t="s">
@@ -36937,7 +37204,7 @@
         <v>452</v>
       </c>
       <c r="B13" s="101" t="s">
-        <v>33</v>
+        <v>508</v>
       </c>
       <c r="C13" s="102" t="s">
         <v>34</v>
@@ -36951,6 +37218,9 @@
       <c r="I13">
         <v>1</v>
       </c>
+      <c r="J13" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="98" t="s">
@@ -36971,6 +37241,9 @@
       <c r="I14">
         <v>1</v>
       </c>
+      <c r="J14" t="s">
+        <v>507</v>
+      </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="102" t="s">
@@ -37011,6 +37284,9 @@
       <c r="I16">
         <v>1</v>
       </c>
+      <c r="J16" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="102" t="s">
@@ -37658,7 +37934,7 @@
       <c r="F47" s="103"/>
       <c r="G47" s="102"/>
     </row>
-    <row r="48" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A48" s="98" t="s">
         <v>483</v>
       </c>
@@ -37748,6 +38024,197 @@
       </c>
       <c r="F52" s="99"/>
       <c r="G52" s="100"/>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>492</v>
+      </c>
+      <c r="B53" t="s">
+        <v>484</v>
+      </c>
+      <c r="C53" t="s">
+        <v>493</v>
+      </c>
+      <c r="D53" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>492</v>
+      </c>
+      <c r="B54" t="s">
+        <v>494</v>
+      </c>
+      <c r="C54" t="s">
+        <v>441</v>
+      </c>
+      <c r="D54" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>492</v>
+      </c>
+      <c r="B55" t="s">
+        <v>496</v>
+      </c>
+      <c r="C55" t="s">
+        <v>444</v>
+      </c>
+      <c r="D55" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>492</v>
+      </c>
+      <c r="B56" t="s">
+        <v>445</v>
+      </c>
+      <c r="C56" t="s">
+        <v>446</v>
+      </c>
+      <c r="D56" t="s">
+        <v>495</v>
+      </c>
+      <c r="E56" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>492</v>
+      </c>
+      <c r="B57" t="s">
+        <v>447</v>
+      </c>
+      <c r="C57" t="s">
+        <v>448</v>
+      </c>
+      <c r="D57" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>492</v>
+      </c>
+      <c r="B58" t="s">
+        <v>490</v>
+      </c>
+      <c r="C58" t="s">
+        <v>491</v>
+      </c>
+      <c r="D58" t="s">
+        <v>495</v>
+      </c>
+      <c r="E58" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>492</v>
+      </c>
+      <c r="B59" t="s">
+        <v>449</v>
+      </c>
+      <c r="C59" t="s">
+        <v>429</v>
+      </c>
+      <c r="D59" t="s">
+        <v>495</v>
+      </c>
+      <c r="E59" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>492</v>
+      </c>
+      <c r="B60" s="107" t="s">
+        <v>138</v>
+      </c>
+      <c r="C60" t="s">
+        <v>138</v>
+      </c>
+      <c r="D60" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>492</v>
+      </c>
+      <c r="B61" t="s">
+        <v>139</v>
+      </c>
+      <c r="C61" t="s">
+        <v>139</v>
+      </c>
+      <c r="D61" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>492</v>
+      </c>
+      <c r="B62" s="107" t="s">
+        <v>140</v>
+      </c>
+      <c r="C62" t="s">
+        <v>140</v>
+      </c>
+      <c r="D62" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>492</v>
+      </c>
+      <c r="B63" t="s">
+        <v>141</v>
+      </c>
+      <c r="C63" t="s">
+        <v>141</v>
+      </c>
+      <c r="D63" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>492</v>
+      </c>
+      <c r="B64" t="s">
+        <v>498</v>
+      </c>
+      <c r="C64" t="s">
+        <v>20</v>
+      </c>
+      <c r="D64" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>492</v>
+      </c>
+      <c r="B65" t="s">
+        <v>499</v>
+      </c>
+      <c r="C65" t="s">
+        <v>500</v>
+      </c>
+      <c r="D65" t="s">
+        <v>495</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -37759,28 +38226,28 @@
   <sheetPr codeName="Sheet5">
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:J294"/>
+  <dimension ref="A1:J296"/>
   <sheetViews>
-    <sheetView topLeftCell="A174" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A195" sqref="A195"/>
+    <sheetView topLeftCell="A272" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A295" sqref="A295:A296"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.1796875" style="71"/>
-    <col min="2" max="2" width="27.81640625" style="69" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.7265625" style="69" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="41.453125" style="69" customWidth="1"/>
-    <col min="5" max="5" width="9.1796875" style="69"/>
-    <col min="6" max="6" width="25.26953125" style="69" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.1796875" style="69"/>
-    <col min="8" max="8" width="10.54296875" style="20" customWidth="1"/>
-    <col min="9" max="9" width="14.1796875" style="20" customWidth="1"/>
-    <col min="10" max="10" width="17.54296875" style="20" customWidth="1"/>
-    <col min="11" max="16384" width="9.1796875" style="20"/>
+    <col min="1" max="1" width="9.109375" style="71"/>
+    <col min="2" max="2" width="27.88671875" style="69" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.6640625" style="69" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="41.44140625" style="69" customWidth="1"/>
+    <col min="5" max="5" width="9.109375" style="69"/>
+    <col min="6" max="6" width="25.33203125" style="69" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.109375" style="69"/>
+    <col min="8" max="8" width="10.5546875" style="20" customWidth="1"/>
+    <col min="9" max="9" width="14.109375" style="20" customWidth="1"/>
+    <col min="10" max="10" width="17.5546875" style="20" customWidth="1"/>
+    <col min="11" max="16384" width="9.109375" style="20"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -40817,7 +41284,7 @@
       </c>
       <c r="J102" s="82"/>
     </row>
-    <row r="103" spans="1:10" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:10" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A103" s="2">
         <v>40101</v>
       </c>
@@ -40934,7 +41401,7 @@
         <v/>
       </c>
     </row>
-    <row r="107" spans="1:10" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:10" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A107" s="9">
         <v>40105</v>
       </c>
@@ -41050,7 +41517,7 @@
         <v/>
       </c>
     </row>
-    <row r="111" spans="1:10" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:10" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A111" s="9">
         <v>40109</v>
       </c>
@@ -45932,7 +46399,7 @@
       </c>
       <c r="J273" s="82"/>
     </row>
-    <row r="274" spans="1:10" ht="13" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A274" s="11">
         <v>59000</v>
       </c>
@@ -45962,7 +46429,7 @@
       </c>
       <c r="J274" s="82"/>
     </row>
-    <row r="275" spans="1:10" ht="13" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A275" s="11">
         <f>A274+1</f>
         <v>59001</v>
@@ -45993,7 +46460,7 @@
       </c>
       <c r="J275" s="82"/>
     </row>
-    <row r="276" spans="1:10" ht="13" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A276" s="11">
         <f>A275+1</f>
         <v>59002</v>
@@ -46024,7 +46491,7 @@
       </c>
       <c r="J276" s="82"/>
     </row>
-    <row r="277" spans="1:10" ht="13" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A277" s="11">
         <f>A276+1</f>
         <v>59003</v>
@@ -46055,7 +46522,7 @@
       </c>
       <c r="J277" s="82"/>
     </row>
-    <row r="278" spans="1:10" ht="13" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A278" s="11">
         <f>A277+1</f>
         <v>59004</v>
@@ -46086,7 +46553,7 @@
       </c>
       <c r="J278" s="82"/>
     </row>
-    <row r="279" spans="1:10" ht="13" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A279" s="11">
         <f>A278+1</f>
         <v>59005</v>
@@ -46549,7 +47016,7 @@
       </c>
       <c r="D294" s="92" t="str">
         <f>IF(VLOOKUP($A294,fields[[code]:[length]],4,FALSE)=0, "", VLOOKUP($A294,fields[[code]:[length]],4,FALSE))</f>
-        <v>החלטה</v>
+        <v>החלטת איחוד</v>
       </c>
       <c r="E294" s="92" t="str">
         <f>IF(VLOOKUP($A294,fields[[code]:[length]],5,FALSE)=0, "", VLOOKUP($A294,fields[[code]:[length]],5,FALSE))</f>
@@ -46561,6 +47028,64 @@
       </c>
       <c r="G294" s="92" t="str">
         <f>IF(VLOOKUP($A294,fields[[code]:[length]],7,FALSE)=0, "", VLOOKUP($A294,fields[[code]:[length]],7,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="295" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A295" s="43">
+        <v>60007</v>
+      </c>
+      <c r="B295" s="92" t="str">
+        <f>IF(VLOOKUP($A295,fields[[code]:[length]],2,FALSE)=0, "", VLOOKUP($A295,fields[[code]:[length]],2,FALSE))</f>
+        <v>unite lines</v>
+      </c>
+      <c r="C295" s="92" t="str">
+        <f>IF(VLOOKUP($A295,fields[[code]:[length]],3,FALSE)=0, "", VLOOKUP($A295,fields[[code]:[length]],3,FALSE))</f>
+        <v>originStand1</v>
+      </c>
+      <c r="D295" s="92" t="str">
+        <f>IF(VLOOKUP($A295,fields[[code]:[length]],4,FALSE)=0, "", VLOOKUP($A295,fields[[code]:[length]],4,FALSE))</f>
+        <v>עומד מקור 1</v>
+      </c>
+      <c r="E295" s="92" t="str">
+        <f>IF(VLOOKUP($A295,fields[[code]:[length]],5,FALSE)=0, "", VLOOKUP($A295,fields[[code]:[length]],5,FALSE))</f>
+        <v>Guid</v>
+      </c>
+      <c r="F295" s="92" t="str">
+        <f>IF(VLOOKUP($A295,fields[[code]:[length]],6,FALSE)=0, "", VLOOKUP($A295,fields[[code]:[length]],6,FALSE))</f>
+        <v/>
+      </c>
+      <c r="G295" s="92" t="str">
+        <f>IF(VLOOKUP($A295,fields[[code]:[length]],7,FALSE)=0, "", VLOOKUP($A295,fields[[code]:[length]],7,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="296" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A296" s="70">
+        <v>60008</v>
+      </c>
+      <c r="B296" s="92" t="str">
+        <f>IF(VLOOKUP($A296,fields[[code]:[length]],2,FALSE)=0, "", VLOOKUP($A296,fields[[code]:[length]],2,FALSE))</f>
+        <v>unite lines</v>
+      </c>
+      <c r="C296" s="92" t="str">
+        <f>IF(VLOOKUP($A296,fields[[code]:[length]],3,FALSE)=0, "", VLOOKUP($A296,fields[[code]:[length]],3,FALSE))</f>
+        <v>originStand2</v>
+      </c>
+      <c r="D296" s="92" t="str">
+        <f>IF(VLOOKUP($A296,fields[[code]:[length]],4,FALSE)=0, "", VLOOKUP($A296,fields[[code]:[length]],4,FALSE))</f>
+        <v>עומד מקור 2</v>
+      </c>
+      <c r="E296" s="92" t="str">
+        <f>IF(VLOOKUP($A296,fields[[code]:[length]],5,FALSE)=0, "", VLOOKUP($A296,fields[[code]:[length]],5,FALSE))</f>
+        <v>Guid</v>
+      </c>
+      <c r="F296" s="92" t="str">
+        <f>IF(VLOOKUP($A296,fields[[code]:[length]],6,FALSE)=0, "", VLOOKUP($A296,fields[[code]:[length]],6,FALSE))</f>
+        <v/>
+      </c>
+      <c r="G296" s="92" t="str">
+        <f>IF(VLOOKUP($A296,fields[[code]:[length]],7,FALSE)=0, "", VLOOKUP($A296,fields[[code]:[length]],7,FALSE))</f>
         <v/>
       </c>
     </row>
@@ -46572,10 +47097,10 @@
       <formula2>9999999999</formula2>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Must be decimal 0 and above" sqref="I2:I4 I6:I287" xr:uid="{41CB88DF-91F0-4D95-8D41-955862E900C8}"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J294" xr:uid="{FB35E6C1-1C83-4856-B6EF-8514E1D19A82}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J296" xr:uid="{FB35E6C1-1C83-4856-B6EF-8514E1D19A82}">
       <formula1>"1"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H294" xr:uid="{2B3AC17D-6DB9-46FC-9461-74329CE0C278}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H296" xr:uid="{2B3AC17D-6DB9-46FC-9461-74329CE0C278}">
       <formula1>"blank,keepValues"</formula1>
     </dataValidation>
   </dataValidations>
@@ -46598,18 +47123,18 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="37.54296875" style="88" customWidth="1"/>
-    <col min="2" max="2" width="35.1796875" style="88" customWidth="1"/>
-    <col min="3" max="3" width="40.26953125" style="88" customWidth="1"/>
-    <col min="4" max="4" width="14.1796875" style="88" customWidth="1"/>
-    <col min="5" max="5" width="17.81640625" style="88" customWidth="1"/>
-    <col min="6" max="6" width="19.26953125" style="88" customWidth="1"/>
+    <col min="1" max="1" width="37.5546875" style="88" customWidth="1"/>
+    <col min="2" max="2" width="35.109375" style="88" customWidth="1"/>
+    <col min="3" max="3" width="40.33203125" style="88" customWidth="1"/>
+    <col min="4" max="4" width="14.109375" style="88" customWidth="1"/>
+    <col min="5" max="5" width="17.88671875" style="88" customWidth="1"/>
+    <col min="6" max="6" width="19.33203125" style="88" customWidth="1"/>
     <col min="7" max="16384" width="10" style="88"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="88" t="s">
         <v>419</v>
       </c>
@@ -46629,7 +47154,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="88" t="str">
         <f>VLOOKUP(D2,fields!A:D,2,FALSE)</f>
         <v>points</v>
@@ -46652,7 +47177,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="88" t="str">
         <f>VLOOKUP(D3,fields!A:D,2,FALSE)</f>
         <v>points</v>
@@ -46675,7 +47200,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="88" t="str">
         <f>VLOOKUP(D4,fields!A:D,2,FALSE)</f>
         <v>points</v>
@@ -46698,7 +47223,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="88" t="str">
         <f>VLOOKUP(D5,fields!A:D,2,FALSE)</f>
         <v>points</v>
@@ -46721,7 +47246,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="88" t="str">
         <f>VLOOKUP(D6,fields!A:D,2,FALSE)</f>
         <v>points</v>
@@ -46744,7 +47269,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="88" t="str">
         <f>VLOOKUP(D7,fields!A:D,2,FALSE)</f>
         <v>points</v>
@@ -46767,7 +47292,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="88" t="str">
         <f>VLOOKUP(D8,fields!A:D,2,FALSE)</f>
         <v>points</v>
@@ -46790,7 +47315,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="88" t="str">
         <f>VLOOKUP(D9,fields!A:D,2,FALSE)</f>
         <v>points</v>
@@ -46813,7 +47338,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="88" t="str">
         <f>VLOOKUP(D10,fields!A:D,2,FALSE)</f>
         <v>points</v>
@@ -46836,7 +47361,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="88" t="str">
         <f>VLOOKUP(D11,fields!A:D,2,FALSE)</f>
         <v>points</v>
@@ -46859,7 +47384,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="88" t="str">
         <f>VLOOKUP(D12,fields!A:D,2,FALSE)</f>
         <v>points</v>
@@ -46882,7 +47407,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="88" t="str">
         <f>VLOOKUP(D13,fields!A:D,2,FALSE)</f>
         <v>points_PlantTypeCoverDistribut</v>
@@ -46905,7 +47430,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="88" t="str">
         <f>VLOOKUP(D14,fields!A:D,2,FALSE)</f>
         <v>points_PlantTypeCoverDistribut</v>
@@ -46928,7 +47453,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="88" t="str">
         <f>VLOOKUP(D15,fields!A:D,2,FALSE)</f>
         <v>points_PlantTypeCoverDistribut</v>
@@ -46951,7 +47476,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="88" t="str">
         <f>VLOOKUP(D16,fields!A:D,2,FALSE)</f>
         <v>points_PlantTypeCoverDistribut</v>
@@ -46974,7 +47499,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="88" t="str">
         <f>VLOOKUP(D17,fields!A:D,2,FALSE)</f>
         <v>points_PlantTypeCoverDistribut</v>
@@ -47017,21 +47542,21 @@
       <selection pane="bottomLeft" activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="8.7265625" style="16"/>
-    <col min="3" max="3" width="8.7265625" style="68"/>
-    <col min="4" max="4" width="13.81640625" style="16" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.81640625" style="16" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.54296875" style="44" customWidth="1"/>
-    <col min="7" max="7" width="31.1796875" style="16" customWidth="1"/>
-    <col min="8" max="8" width="19.1796875" style="16" customWidth="1"/>
-    <col min="9" max="9" width="25.7265625" style="16" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="23.7265625" style="46" customWidth="1"/>
-    <col min="11" max="16384" width="8.7265625" style="16"/>
+    <col min="1" max="2" width="8.6640625" style="16"/>
+    <col min="3" max="3" width="8.6640625" style="68"/>
+    <col min="4" max="4" width="13.88671875" style="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.88671875" style="16" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.5546875" style="44" customWidth="1"/>
+    <col min="7" max="7" width="31.109375" style="16" customWidth="1"/>
+    <col min="8" max="8" width="19.109375" style="16" customWidth="1"/>
+    <col min="9" max="9" width="25.6640625" style="16" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.6640625" style="46" customWidth="1"/>
+    <col min="11" max="16384" width="8.6640625" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>1</v>
       </c>
@@ -47383,7 +47908,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:10" s="20" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="43">
         <v>50027</v>
       </c>
@@ -47491,7 +48016,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="1:10" s="20" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="43">
         <v>50028</v>
       </c>
@@ -47739,7 +48264,7 @@
       <c r="I26" s="16"/>
       <c r="J26" s="46"/>
     </row>
-    <row r="27" spans="1:10" s="20" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="43">
         <v>50039</v>
       </c>
@@ -47827,7 +48352,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="30" spans="1:10" s="20" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="43">
         <v>50037</v>
       </c>
@@ -47857,7 +48382,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="31" spans="1:10" s="20" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="43">
         <v>50041</v>
       </c>
@@ -47917,7 +48442,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="33" spans="1:10" s="20" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="43">
         <v>50042</v>
       </c>
@@ -47947,7 +48472,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="34" spans="1:10" s="20" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="43">
         <v>50044</v>
       </c>
@@ -48007,7 +48532,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="36" spans="1:10" s="20" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="43">
         <v>50043</v>
       </c>
@@ -48037,7 +48562,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="37" spans="1:10" s="20" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="43">
         <v>50032</v>
       </c>
@@ -48065,7 +48590,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="38" spans="1:10" s="20" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="43">
         <v>50030</v>
       </c>
@@ -48095,7 +48620,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="39" spans="1:10" s="20" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="43">
         <v>50029</v>
       </c>
@@ -48125,7 +48650,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="40" spans="1:10" s="20" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="43">
         <v>50031</v>
       </c>
@@ -48155,7 +48680,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="41" spans="1:10" s="20" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="43">
         <v>50036</v>
       </c>
@@ -48183,7 +48708,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="42" spans="1:10" s="20" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="43">
         <v>50034</v>
       </c>
@@ -48213,7 +48738,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="43" spans="1:10" s="20" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="43">
         <v>50033</v>
       </c>
@@ -48243,7 +48768,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="44" spans="1:10" s="20" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="43">
         <v>50035</v>
       </c>
@@ -48273,7 +48798,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="45" spans="1:10" s="20" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="43">
         <v>50046</v>
       </c>
@@ -48301,7 +48826,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="46" spans="1:10" s="20" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="43">
         <v>50047</v>
       </c>
@@ -48331,7 +48856,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="47" spans="1:10" s="20" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="43">
         <v>50049</v>
       </c>
@@ -48359,7 +48884,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="48" spans="1:10" s="20" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="43">
         <v>50048</v>
       </c>
@@ -48387,7 +48912,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="49" spans="1:10" s="20" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="43">
         <v>50050</v>
       </c>
@@ -48415,7 +48940,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="50" spans="1:10" s="20" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="43">
         <v>50051</v>
       </c>
@@ -48445,7 +48970,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="51" spans="1:10" s="20" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="43">
         <v>50053</v>
       </c>
@@ -48473,7 +48998,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="52" spans="1:10" s="20" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="43">
         <v>50052</v>
       </c>
@@ -48501,7 +49026,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="53" spans="1:10" s="20" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="43">
         <v>50054</v>
       </c>
@@ -48529,7 +49054,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="54" spans="1:10" s="20" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="43">
         <v>50055</v>
       </c>
@@ -48559,7 +49084,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="55" spans="1:10" s="20" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="43">
         <v>50057</v>
       </c>
@@ -48587,7 +49112,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="56" spans="1:10" s="20" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="43">
         <v>50056</v>
       </c>
@@ -48615,7 +49140,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="57" spans="1:10" s="20" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="43">
         <v>50058</v>
       </c>
@@ -48643,7 +49168,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="58" spans="1:10" s="20" customFormat="1" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" s="20" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A58" s="43">
         <v>50089</v>
       </c>
@@ -48673,7 +49198,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="59" spans="1:10" s="20" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="43">
         <v>50060</v>
       </c>
@@ -48701,7 +49226,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="60" spans="1:10" s="20" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="43">
         <v>50059</v>
       </c>
@@ -48785,7 +49310,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="63" spans="1:10" s="20" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="43">
         <v>50063</v>
       </c>
@@ -48815,7 +49340,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="64" spans="1:10" s="20" customFormat="1" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:10" s="20" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A64" s="43">
         <v>50064</v>
       </c>
@@ -48845,7 +49370,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="65" spans="1:10" s="20" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="43">
         <v>50065</v>
       </c>
@@ -48875,7 +49400,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="66" spans="1:10" s="20" customFormat="1" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:10" s="20" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A66" s="43">
         <v>50066</v>
       </c>
@@ -48905,7 +49430,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="67" spans="1:10" s="20" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="43">
         <v>50102</v>
       </c>
@@ -48933,7 +49458,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="68" spans="1:10" s="20" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="43">
         <v>50068</v>
       </c>
@@ -48963,7 +49488,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="69" spans="1:10" s="20" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="43">
         <v>50069</v>
       </c>
@@ -48993,7 +49518,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="70" spans="1:10" s="20" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="43">
         <v>50070</v>
       </c>
@@ -49023,7 +49548,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="71" spans="1:10" s="20" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="43">
         <v>50071</v>
       </c>
@@ -49053,7 +49578,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="72" spans="1:10" s="20" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="43">
         <v>50067</v>
       </c>
@@ -49083,7 +49608,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="73" spans="1:10" s="20" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="43">
         <v>50072</v>
       </c>
@@ -49113,7 +49638,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="74" spans="1:10" s="20" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="43">
         <v>50073</v>
       </c>
@@ -49141,7 +49666,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="75" spans="1:10" s="20" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="43">
         <v>50074</v>
       </c>
@@ -49169,7 +49694,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="76" spans="1:10" s="20" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="43">
         <v>50075</v>
       </c>
@@ -49225,7 +49750,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="78" spans="1:10" s="20" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" s="43">
         <v>50076</v>
       </c>
@@ -49253,7 +49778,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="79" spans="1:10" s="20" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79" s="43">
         <v>50104</v>
       </c>
@@ -49281,7 +49806,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="80" spans="1:10" s="20" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A80" s="43">
         <v>50077</v>
       </c>
@@ -49309,7 +49834,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="81" spans="1:10" s="20" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="43">
         <v>50105</v>
       </c>
@@ -49337,7 +49862,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="82" spans="1:10" s="20" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A82" s="43">
         <v>50078</v>
       </c>
@@ -49365,7 +49890,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="83" spans="1:10" s="20" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" s="43">
         <v>50106</v>
       </c>
@@ -49778,7 +50303,7 @@
       <c r="I102" s="19"/>
       <c r="J102" s="19"/>
     </row>
-    <row r="103" spans="1:10" s="20" customFormat="1" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:10" s="20" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A103" s="17">
         <v>40017</v>
       </c>
@@ -49866,7 +50391,7 @@
       </c>
       <c r="J106" s="19"/>
     </row>
-    <row r="107" spans="1:10" s="20" customFormat="1" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:10" s="20" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A107" s="33">
         <v>40021</v>
       </c>
@@ -49955,7 +50480,7 @@
       <c r="I110" s="19"/>
       <c r="J110" s="19"/>
     </row>
-    <row r="111" spans="1:10" s="20" customFormat="1" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:10" s="20" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A111" s="33">
         <v>40025</v>
       </c>
@@ -51031,7 +51556,7 @@
       <c r="I162" s="19"/>
       <c r="J162" s="19"/>
     </row>
-    <row r="163" spans="1:10" ht="14.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:10" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A163" s="17">
         <v>40077</v>
       </c>
@@ -51053,7 +51578,7 @@
       <c r="I163" s="19"/>
       <c r="J163" s="19"/>
     </row>
-    <row r="164" spans="1:10" ht="14.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:10" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A164" s="17">
         <v>40078</v>
       </c>
@@ -51075,7 +51600,7 @@
       <c r="I164" s="19"/>
       <c r="J164" s="19"/>
     </row>
-    <row r="165" spans="1:10" ht="14.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:10" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A165" s="17">
         <v>40079</v>
       </c>
@@ -51097,7 +51622,7 @@
       <c r="I165" s="19"/>
       <c r="J165" s="19"/>
     </row>
-    <row r="166" spans="1:10" ht="12.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A166" s="17">
         <v>40080</v>
       </c>
@@ -51119,7 +51644,7 @@
       <c r="I166" s="19"/>
       <c r="J166" s="19"/>
     </row>
-    <row r="167" spans="1:10" ht="12.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A167" s="17">
         <v>40081</v>
       </c>
@@ -51141,7 +51666,7 @@
       <c r="I167" s="19"/>
       <c r="J167" s="19"/>
     </row>
-    <row r="168" spans="1:10" ht="12.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A168" s="17">
         <v>40082</v>
       </c>
@@ -51165,7 +51690,7 @@
       <c r="I168" s="19"/>
       <c r="J168" s="19"/>
     </row>
-    <row r="169" spans="1:10" ht="12.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A169" s="17">
         <v>40083</v>
       </c>
@@ -51187,7 +51712,7 @@
       <c r="I169" s="19"/>
       <c r="J169" s="19"/>
     </row>
-    <row r="170" spans="1:10" ht="14.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:10" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A170" s="17">
         <v>40084</v>
       </c>
@@ -51209,7 +51734,7 @@
       <c r="I170" s="19"/>
       <c r="J170" s="19"/>
     </row>
-    <row r="171" spans="1:10" ht="14.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:10" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A171" s="17">
         <v>40085</v>
       </c>
@@ -51231,7 +51756,7 @@
       <c r="I171" s="19"/>
       <c r="J171" s="19"/>
     </row>
-    <row r="172" spans="1:10" ht="14.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:10" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A172" s="17">
         <v>40086</v>
       </c>
@@ -51253,7 +51778,7 @@
       <c r="I172" s="19"/>
       <c r="J172" s="19"/>
     </row>
-    <row r="173" spans="1:10" ht="14.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:10" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A173" s="17">
         <v>40087</v>
       </c>
@@ -51297,7 +51822,7 @@
       <c r="I174" s="19"/>
       <c r="J174" s="19"/>
     </row>
-    <row r="175" spans="1:10" ht="14.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:10" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A175" s="17">
         <v>40089</v>
       </c>
@@ -51341,7 +51866,7 @@
       <c r="I176" s="19"/>
       <c r="J176" s="19"/>
     </row>
-    <row r="177" spans="1:10" ht="12.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A177" s="17">
         <v>40091</v>
       </c>
@@ -51363,7 +51888,7 @@
       <c r="I177" s="19"/>
       <c r="J177" s="19"/>
     </row>
-    <row r="178" spans="1:10" ht="12.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A178" s="17">
         <v>40092</v>
       </c>
@@ -51385,7 +51910,7 @@
       <c r="I178" s="19"/>
       <c r="J178" s="19"/>
     </row>
-    <row r="179" spans="1:10" ht="12.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A179" s="17">
         <v>40093</v>
       </c>
@@ -51407,7 +51932,7 @@
       <c r="I179" s="19"/>
       <c r="J179" s="19"/>
     </row>
-    <row r="180" spans="1:10" ht="12.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A180" s="17">
         <v>40094</v>
       </c>
@@ -51429,7 +51954,7 @@
       <c r="I180" s="19"/>
       <c r="J180" s="19"/>
     </row>
-    <row r="181" spans="1:10" ht="12.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A181" s="17">
         <v>40095</v>
       </c>
@@ -51451,7 +51976,7 @@
       <c r="I181" s="19"/>
       <c r="J181" s="19"/>
     </row>
-    <row r="182" spans="1:10" ht="12.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A182" s="17">
         <v>40096</v>
       </c>
@@ -51473,7 +51998,7 @@
       <c r="I182" s="19"/>
       <c r="J182" s="19"/>
     </row>
-    <row r="183" spans="1:10" ht="12.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A183" s="17">
         <v>40097</v>
       </c>
@@ -51495,7 +52020,7 @@
       <c r="I183" s="19"/>
       <c r="J183" s="19"/>
     </row>
-    <row r="184" spans="1:10" s="59" customFormat="1" ht="12.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:10" s="59" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A184" s="17">
         <v>40098</v>
       </c>
@@ -51517,7 +52042,7 @@
       <c r="I184" s="19"/>
       <c r="J184" s="19"/>
     </row>
-    <row r="185" spans="1:10" ht="12.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A185" s="17">
         <v>40099</v>
       </c>
@@ -51539,7 +52064,7 @@
       <c r="I185" s="19"/>
       <c r="J185" s="19"/>
     </row>
-    <row r="186" spans="1:10" ht="12.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A186" s="17">
         <v>40100</v>
       </c>
@@ -51561,7 +52086,7 @@
       <c r="I186" s="19"/>
       <c r="J186" s="19"/>
     </row>
-    <row r="187" spans="1:10" ht="12.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A187" s="17">
         <v>40101</v>
       </c>
@@ -51583,7 +52108,7 @@
       <c r="I187" s="19"/>
       <c r="J187" s="19"/>
     </row>
-    <row r="188" spans="1:10" ht="12.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A188" s="17">
         <v>40102</v>
       </c>
@@ -51607,7 +52132,7 @@
       <c r="I188" s="19"/>
       <c r="J188" s="19"/>
     </row>
-    <row r="189" spans="1:10" ht="12.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A189" s="17">
         <v>40103</v>
       </c>
@@ -51631,7 +52156,7 @@
       <c r="I189" s="19"/>
       <c r="J189" s="19"/>
     </row>
-    <row r="190" spans="1:10" ht="12.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A190" s="17">
         <v>40104</v>
       </c>
@@ -51655,7 +52180,7 @@
       <c r="I190" s="19"/>
       <c r="J190" s="19"/>
     </row>
-    <row r="191" spans="1:10" ht="12.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A191" s="17">
         <v>40105</v>
       </c>
@@ -51679,7 +52204,7 @@
       <c r="I191" s="19"/>
       <c r="J191" s="19"/>
     </row>
-    <row r="192" spans="1:10" ht="12.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A192" s="17">
         <v>40106</v>
       </c>
@@ -51703,7 +52228,7 @@
       <c r="I192" s="19"/>
       <c r="J192" s="19"/>
     </row>
-    <row r="193" spans="1:10" ht="12.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A193" s="17">
         <v>40107</v>
       </c>
@@ -51727,7 +52252,7 @@
       <c r="I193" s="19"/>
       <c r="J193" s="19"/>
     </row>
-    <row r="194" spans="1:10" ht="13" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:10" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A194" s="17">
         <v>40108</v>
       </c>
@@ -51751,7 +52276,7 @@
       <c r="I194" s="19"/>
       <c r="J194" s="19"/>
     </row>
-    <row r="195" spans="1:10" ht="13" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:10" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A195" s="17">
         <v>40109</v>
       </c>
@@ -51775,7 +52300,7 @@
       <c r="I195" s="19"/>
       <c r="J195" s="19"/>
     </row>
-    <row r="196" spans="1:10" ht="13" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:10" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A196" s="17">
         <v>40110</v>
       </c>
@@ -51797,7 +52322,7 @@
       <c r="I196" s="19"/>
       <c r="J196" s="19"/>
     </row>
-    <row r="197" spans="1:10" ht="13" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:10" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A197" s="17">
         <v>40111</v>
       </c>
@@ -51819,7 +52344,7 @@
       <c r="I197" s="19"/>
       <c r="J197" s="19"/>
     </row>
-    <row r="198" spans="1:10" ht="13" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:10" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A198" s="17">
         <v>40112</v>
       </c>
@@ -51841,7 +52366,7 @@
       <c r="I198" s="19"/>
       <c r="J198" s="19"/>
     </row>
-    <row r="199" spans="1:10" ht="13" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:10" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A199" s="17">
         <v>40113</v>
       </c>
@@ -51863,7 +52388,7 @@
       <c r="I199" s="19"/>
       <c r="J199" s="19"/>
     </row>
-    <row r="200" spans="1:10" ht="13" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:10" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A200" s="17">
         <v>40114</v>
       </c>
@@ -52137,7 +52662,7 @@
       <c r="I211" s="19"/>
       <c r="J211" s="19"/>
     </row>
-    <row r="212" spans="1:10" ht="13" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:10" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A212" s="38">
         <v>41007</v>
       </c>
@@ -52251,7 +52776,7 @@
       </c>
       <c r="J216" s="18"/>
     </row>
-    <row r="217" spans="1:10" ht="13" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:10" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A217" s="39">
         <v>42003</v>
       </c>
@@ -52321,7 +52846,7 @@
       <c r="I219" s="19"/>
       <c r="J219" s="19"/>
     </row>
-    <row r="220" spans="1:10" ht="13" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:10" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A220" s="39">
         <v>42006</v>
       </c>
@@ -52343,7 +52868,7 @@
       <c r="I220" s="19"/>
       <c r="J220" s="19"/>
     </row>
-    <row r="221" spans="1:10" ht="13" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:10" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A221" s="39">
         <v>42007</v>
       </c>
@@ -52387,7 +52912,7 @@
       <c r="I222" s="19"/>
       <c r="J222" s="19"/>
     </row>
-    <row r="223" spans="1:10" ht="13" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:10" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A223" s="40">
         <v>43000</v>
       </c>
@@ -52409,7 +52934,7 @@
       <c r="I223" s="19"/>
       <c r="J223" s="19"/>
     </row>
-    <row r="224" spans="1:10" ht="13" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:10" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A224" s="40">
         <v>43001</v>
       </c>
@@ -52431,7 +52956,7 @@
       <c r="I224" s="19"/>
       <c r="J224" s="19"/>
     </row>
-    <row r="225" spans="1:10" ht="13" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:10" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A225" s="40">
         <v>43002</v>
       </c>
@@ -52453,7 +52978,7 @@
       <c r="I225" s="19"/>
       <c r="J225" s="19"/>
     </row>
-    <row r="226" spans="1:10" ht="13" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:10" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A226" s="40">
         <v>43003</v>
       </c>
@@ -52475,7 +53000,7 @@
       <c r="I226" s="19"/>
       <c r="J226" s="19"/>
     </row>
-    <row r="227" spans="1:10" ht="13" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:10" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A227" s="40">
         <v>43004</v>
       </c>
@@ -52497,7 +53022,7 @@
       <c r="I227" s="19"/>
       <c r="J227" s="19"/>
     </row>
-    <row r="228" spans="1:10" ht="13" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:10" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A228" s="40">
         <v>43005</v>
       </c>
@@ -52637,7 +53162,7 @@
       <c r="I233" s="19"/>
       <c r="J233" s="19"/>
     </row>
-    <row r="234" spans="1:10" ht="13" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:10" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A234" s="40">
         <v>43011</v>
       </c>
@@ -52681,7 +53206,7 @@
       <c r="I235" s="19"/>
       <c r="J235" s="19"/>
     </row>
-    <row r="236" spans="1:10" ht="13" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:10" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A236" s="40">
         <v>43013</v>
       </c>
@@ -52703,7 +53228,7 @@
       <c r="I236" s="19"/>
       <c r="J236" s="19"/>
     </row>
-    <row r="237" spans="1:10" ht="13" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:10" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A237" s="41">
         <v>44000</v>
       </c>
@@ -52725,7 +53250,7 @@
       <c r="I237" s="19"/>
       <c r="J237" s="19"/>
     </row>
-    <row r="238" spans="1:10" ht="13" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:10" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A238" s="41">
         <v>44001</v>
       </c>
@@ -52747,7 +53272,7 @@
       <c r="I238" s="19"/>
       <c r="J238" s="19"/>
     </row>
-    <row r="239" spans="1:10" ht="13" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:10" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A239" s="41">
         <v>44002</v>
       </c>
@@ -52773,7 +53298,7 @@
       </c>
       <c r="J239" s="19"/>
     </row>
-    <row r="240" spans="1:10" ht="13" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:10" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A240" s="41">
         <v>44003</v>
       </c>
@@ -52799,7 +53324,7 @@
       </c>
       <c r="J240" s="18"/>
     </row>
-    <row r="241" spans="1:10" ht="13" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:10" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A241" s="41">
         <v>44004</v>
       </c>
@@ -52821,7 +53346,7 @@
       <c r="I241" s="19"/>
       <c r="J241" s="19"/>
     </row>
-    <row r="242" spans="1:10" ht="13" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:10" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A242" s="41">
         <v>44005</v>
       </c>
@@ -52843,7 +53368,7 @@
       <c r="I242" s="19"/>
       <c r="J242" s="19"/>
     </row>
-    <row r="243" spans="1:10" ht="13" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:10" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A243" s="41">
         <v>44006</v>
       </c>
@@ -52865,7 +53390,7 @@
       <c r="I243" s="19"/>
       <c r="J243" s="19"/>
     </row>
-    <row r="244" spans="1:10" ht="13" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:10" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A244" s="41">
         <v>44007</v>
       </c>
@@ -52887,7 +53412,7 @@
       <c r="I244" s="19"/>
       <c r="J244" s="19"/>
     </row>
-    <row r="245" spans="1:10" ht="13" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:10" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A245" s="41">
         <v>44008</v>
       </c>
@@ -52909,7 +53434,7 @@
       <c r="I245" s="19"/>
       <c r="J245" s="19"/>
     </row>
-    <row r="246" spans="1:10" ht="13" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:10" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A246" s="43">
         <v>50023</v>
       </c>
@@ -52926,7 +53451,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="247" spans="1:10" ht="13" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:10" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A247" s="43">
         <v>50001</v>
       </c>
@@ -52943,7 +53468,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="248" spans="1:10" ht="13" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:10" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A248" s="43">
         <v>50024</v>
       </c>
@@ -52960,7 +53485,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="249" spans="1:10" ht="13" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:10" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A249" s="43">
         <v>50101</v>
       </c>
@@ -52982,7 +53507,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="250" spans="1:10" ht="13" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:10" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A250" s="43">
         <v>50000</v>
       </c>
@@ -53206,7 +53731,7 @@
       </c>
       <c r="I261" s="16"/>
     </row>
-    <row r="262" spans="1:9" s="20" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A262" s="65">
         <v>59000</v>
       </c>
@@ -53226,7 +53751,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="263" spans="1:9" s="20" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A263" s="65">
         <f>A262+1</f>
         <v>59001</v>
@@ -53247,7 +53772,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="264" spans="1:9" s="20" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A264" s="65">
         <f>A263+1</f>
         <v>59002</v>
@@ -53268,7 +53793,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="265" spans="1:9" s="20" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A265" s="65">
         <f>A264+1</f>
         <v>59003</v>
@@ -53289,7 +53814,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="266" spans="1:9" s="20" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A266" s="65">
         <f>A265+1</f>
         <v>59004</v>
@@ -53310,7 +53835,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="267" spans="1:9" s="20" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A267" s="65">
         <f>A266+1</f>
         <v>59005</v>
@@ -53540,7 +54065,7 @@
       </c>
       <c r="I276" s="16"/>
     </row>
-    <row r="277" spans="1:9" s="46" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:9" s="46" customFormat="1" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A277" s="43">
         <v>50020</v>
       </c>
@@ -53582,7 +54107,7 @@
       </c>
       <c r="I278" s="16"/>
     </row>
-    <row r="279" spans="1:9" s="46" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:9" s="46" customFormat="1" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A279" s="43">
         <v>50022</v>
       </c>
@@ -53603,7 +54128,7 @@
       </c>
       <c r="I279" s="16"/>
     </row>
-    <row r="280" spans="1:9" s="46" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:9" s="46" customFormat="1" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A280" s="43">
         <v>50025</v>
       </c>
@@ -53624,7 +54149,7 @@
       </c>
       <c r="I280" s="16"/>
     </row>
-    <row r="281" spans="1:9" s="46" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:9" s="46" customFormat="1" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A281" s="43">
         <v>50026</v>
       </c>

</xml_diff>

<commit_message>
Updating field names in a fields file
</commit_message>
<xml_diff>
--- a/DesheTools/configuration/fields.xlsx
+++ b/DesheTools/configuration/fields.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\galisraeli\Documents\GitHub\Deshe\DesheTools\configuration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5D5F4BE-0200-42D2-8448-06908350019C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ECF0B23-6439-421F-9A2B-17EEDE20C926}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="642" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36948,8 +36948,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B206E146-10D4-4101-A6FA-71BD0AF9A72C}">
   <dimension ref="A1:J65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -37227,7 +37227,7 @@
         <v>452</v>
       </c>
       <c r="B14" s="105" t="s">
-        <v>453</v>
+        <v>507</v>
       </c>
       <c r="C14" s="98" t="s">
         <v>454</v>
@@ -37242,7 +37242,7 @@
         <v>1</v>
       </c>
       <c r="J14" t="s">
-        <v>507</v>
+        <v>453</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -37678,7 +37678,7 @@
         <v>1</v>
       </c>
       <c r="J35" s="107" t="s">
-        <v>453</v>
+        <v>507</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>